<commit_message>
Fill status fixes and other bug fixes
</commit_message>
<xml_diff>
--- a/export2.xlsx
+++ b/export2.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="3" autoFilterDateGrouping="1" firstSheet="3" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="13665" windowWidth="26775" xWindow="29010" yWindow="2280"/>
+    <workbookView activeTab="3" autoFilterDateGrouping="1" firstSheet="3" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-120" yWindow="480"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="tblAdditionalInfo" sheetId="1" state="veryHidden" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="tblTabsOrder" sheetId="2" state="veryHidden" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bid Breakdown_MetaData" sheetId="3" state="veryHidden" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Bid Breakdown" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="153">
   <si>
     <t>tblAdditionalInfo</t>
   </si>
@@ -332,6 +333,9 @@
   </si>
   <si>
     <t>Bid Item:  || Base Bid</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
   <si>
     <t xml:space="preserve"> || Electrical Utility</t>
@@ -1728,7 +1732,7 @@
   <dimension ref="A1:AF50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="AE1" sqref="AE1:AF1048576"/>
+      <selection activeCell="X1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75" outlineLevelCol="0"/>
@@ -1935,18 +1939,16 @@
       <c r="Z3" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="AE3" s="7">
-        <f>Q2/P2</f>
-        <v/>
-      </c>
-      <c r="AF3" s="7">
-        <f>P2/Z2</f>
-        <v/>
+      <c r="AE3" s="7" t="n">
+        <v>78.77419321349434</v>
+      </c>
+      <c r="AF3" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:32">
       <c r="B4" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>17718.49</v>
@@ -1991,20 +1993,18 @@
         <v>1312.4</v>
       </c>
       <c r="AD4" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE4" s="7">
-        <f>Q3/P3</f>
-        <v/>
-      </c>
-      <c r="AF4" s="7">
-        <f>P3/Z3</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE4" s="7" t="n">
+        <v>86.04350827191556</v>
+      </c>
+      <c r="AF4" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:32">
       <c r="B5" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>23082.52</v>
@@ -2049,20 +2049,18 @@
         <v>1709.82</v>
       </c>
       <c r="AD5" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE5" s="7">
-        <f>Q4/P4</f>
-        <v/>
-      </c>
-      <c r="AF5" s="7">
-        <f>P4/Z4</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE5" s="7" t="n">
+        <v>92.61043485445182</v>
+      </c>
+      <c r="AF5" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:32">
       <c r="B6" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C6" s="2" t="n">
         <v>10858.15</v>
@@ -2107,20 +2105,18 @@
         <v>804.3099999999999</v>
       </c>
       <c r="AD6" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE6" s="7">
-        <f>Q5/P5</f>
-        <v/>
-      </c>
-      <c r="AF6" s="7">
-        <f>P5/Z5</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE6" s="7" t="n">
+        <v>79.21492738362883</v>
+      </c>
+      <c r="AF6" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:32">
       <c r="B7" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C7" s="2" t="n">
         <v>33420.73</v>
@@ -2165,20 +2161,18 @@
         <v>2475.61</v>
       </c>
       <c r="AD7" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE7" s="7">
-        <f>Q6/P6</f>
-        <v/>
-      </c>
-      <c r="AF7" s="7">
-        <f>P6/Z6</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE7" s="7" t="n">
+        <v>76.39629826788421</v>
+      </c>
+      <c r="AF7" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:32">
       <c r="B8" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C8" s="2" t="n">
         <v>343502.09</v>
@@ -2226,20 +2220,18 @@
         <v>25444.6</v>
       </c>
       <c r="AD8" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE8" s="7">
-        <f>Q7/P7</f>
-        <v/>
-      </c>
-      <c r="AF8" s="7">
-        <f>P7/Z7</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE8" s="7" t="n">
+        <v>76.46518480642565</v>
+      </c>
+      <c r="AF8" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:32">
       <c r="B9" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C9" s="2" t="n">
         <v>271072.05</v>
@@ -2284,20 +2276,18 @@
         <v>20079.41</v>
       </c>
       <c r="AD9" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE9" s="7">
-        <f>Q8/P8</f>
-        <v/>
-      </c>
-      <c r="AF9" s="7">
-        <f>P8/Z8</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE9" s="7" t="n">
+        <v>80.78043677142801</v>
+      </c>
+      <c r="AF9" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:32">
       <c r="B10" s="1" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C10" s="2" t="n">
         <v>2554.74</v>
@@ -2342,20 +2332,18 @@
         <v>189.24</v>
       </c>
       <c r="AD10" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE10" s="7">
-        <f>Q9/P9</f>
-        <v/>
-      </c>
-      <c r="AF10" s="7">
-        <f>P9/Z9</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE10" s="7" t="n">
+        <v>76.5871757925072</v>
+      </c>
+      <c r="AF10" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:32">
       <c r="B11" s="1" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C11" s="2" t="n">
         <v>134628.47</v>
@@ -2403,20 +2391,18 @@
         <v>9972.48</v>
       </c>
       <c r="AD11" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE11" s="7">
-        <f>Q10/P10</f>
-        <v/>
-      </c>
-      <c r="AF11" s="7">
-        <f>P10/Z10</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE11" s="7" t="n">
+        <v>78.94320730795488</v>
+      </c>
+      <c r="AF11" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:32">
       <c r="B12" s="1" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C12" s="2" t="n">
         <v>13088.93</v>
@@ -2461,20 +2447,18 @@
         <v>969.55</v>
       </c>
       <c r="AD12" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE12" s="7">
-        <f>Q11/P11</f>
-        <v/>
-      </c>
-      <c r="AF12" s="7">
-        <f>P11/Z11</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE12" s="7" t="n">
+        <v>86.97506982517844</v>
+      </c>
+      <c r="AF12" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:32">
       <c r="B13" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C13" s="2" t="n">
         <v>507457.26</v>
@@ -2519,20 +2503,18 @@
         <v>37589.43</v>
       </c>
       <c r="AD13" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE13" s="7">
-        <f>Q12/P12</f>
-        <v/>
-      </c>
-      <c r="AF13" s="7">
-        <f>P12/Z12</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE13" s="7" t="n">
+        <v>81.76436600647931</v>
+      </c>
+      <c r="AF13" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:32">
       <c r="B14" s="1" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C14" s="2" t="n">
         <v>2926.41</v>
@@ -2577,20 +2559,18 @@
         <v>216.77</v>
       </c>
       <c r="AD14" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE14" s="7">
-        <f>Q13/P13</f>
-        <v/>
-      </c>
-      <c r="AF14" s="7">
-        <f>P13/Z13</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE14" s="7" t="n">
+        <v>85.44885361552028</v>
+      </c>
+      <c r="AF14" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:32">
       <c r="B15" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C15" s="2" t="n">
         <v>73400.10000000001</v>
@@ -2635,20 +2615,18 @@
         <v>5437.04</v>
       </c>
       <c r="AD15" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE15" s="7">
-        <f>Q14/P14</f>
-        <v/>
-      </c>
-      <c r="AF15" s="7">
-        <f>P14/Z14</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE15" s="7" t="n">
+        <v>86.45063055901883</v>
+      </c>
+      <c r="AF15" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:32">
       <c r="B16" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>795517.4300000001</v>
@@ -2696,20 +2674,18 @@
         <v>58927.22</v>
       </c>
       <c r="AD16" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE16" s="7">
-        <f>Q15/P15</f>
-        <v/>
-      </c>
-      <c r="AF16" s="7">
-        <f>P15/Z15</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE16" s="7" t="n">
+        <v>80.05861580031198</v>
+      </c>
+      <c r="AF16" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:32">
       <c r="B17" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C17" s="2" t="n">
         <v>25277.84</v>
@@ -2754,20 +2730,18 @@
         <v>1872.43</v>
       </c>
       <c r="AD17" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE17" s="7">
-        <f>Q16/P16</f>
-        <v/>
-      </c>
-      <c r="AF17" s="7">
-        <f>P16/Z16</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE17" s="7" t="n">
+        <v>79.28473065025601</v>
+      </c>
+      <c r="AF17" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="18" spans="1:32">
       <c r="B18" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C18" s="2" t="n">
         <v>118152.69</v>
@@ -2812,20 +2786,18 @@
         <v>8752.049999999999</v>
       </c>
       <c r="AD18" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE18" s="7">
-        <f>Q17/P17</f>
-        <v/>
-      </c>
-      <c r="AF18" s="7">
-        <f>P17/Z17</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE18" s="7" t="n">
+        <v>81.3509519749929</v>
+      </c>
+      <c r="AF18" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="19" spans="1:32">
       <c r="B19" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C19" s="2" t="n">
         <v>1486389.63</v>
@@ -2873,20 +2845,18 @@
         <v>110102.94</v>
       </c>
       <c r="AD19" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE19" s="7">
-        <f>Q18/P18</f>
-        <v/>
-      </c>
-      <c r="AF19" s="7">
-        <f>P18/Z18</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE19" s="7" t="n">
+        <v>76.38777747603218</v>
+      </c>
+      <c r="AF19" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:32">
       <c r="B20" s="1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C20" s="2" t="n">
         <v>154142.46</v>
@@ -2934,20 +2904,18 @@
         <v>11417.96</v>
       </c>
       <c r="AD20" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE20" s="7">
-        <f>Q19/P19</f>
-        <v/>
-      </c>
-      <c r="AF20" s="7">
-        <f>P19/Z19</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE20" s="7" t="n">
+        <v>79.12129991855483</v>
+      </c>
+      <c r="AF20" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="21" spans="1:32">
       <c r="B21" s="1" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C21" s="2" t="n">
         <v>651704.13</v>
@@ -2995,20 +2963,18 @@
         <v>48274.38</v>
       </c>
       <c r="AD21" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE21" s="7">
-        <f>Q20/P20</f>
-        <v/>
-      </c>
-      <c r="AF21" s="7">
-        <f>P20/Z20</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE21" s="7" t="n">
+        <v>80.25944267144723</v>
+      </c>
+      <c r="AF21" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:32">
       <c r="B22" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C22" s="2" t="n">
         <v>674025.4399999999</v>
@@ -3056,20 +3022,18 @@
         <v>49927.81</v>
       </c>
       <c r="AD22" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE22" s="7">
-        <f>Q21/P21</f>
-        <v/>
-      </c>
-      <c r="AF22" s="7">
-        <f>P21/Z21</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE22" s="7" t="n">
+        <v>77.00658576079354</v>
+      </c>
+      <c r="AF22" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:32">
       <c r="B23" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C23" s="2" t="n">
         <v>34851.06</v>
@@ -3117,20 +3081,18 @@
         <v>2581.56</v>
       </c>
       <c r="AD23" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE23" s="7">
-        <f>Q22/P22</f>
-        <v/>
-      </c>
-      <c r="AF23" s="7">
-        <f>P22/Z22</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE23" s="7" t="n">
+        <v>76.56259677551871</v>
+      </c>
+      <c r="AF23" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:32">
       <c r="B24" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C24" s="2" t="n">
         <v>1471.74</v>
@@ -3175,20 +3137,18 @@
         <v>109.02</v>
       </c>
       <c r="AD24" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE24" s="7">
-        <f>Q23/P23</f>
-        <v/>
-      </c>
-      <c r="AF24" s="7">
-        <f>P23/Z23</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE24" s="7" t="n">
+        <v>77.99481072450268</v>
+      </c>
+      <c r="AF24" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:32">
       <c r="B25" s="1" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C25" s="2" t="n">
         <v>58762.25</v>
@@ -3236,20 +3196,18 @@
         <v>4352.76</v>
       </c>
       <c r="AD25" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE25" s="7">
-        <f>Q24/P24</f>
-        <v/>
-      </c>
-      <c r="AF25" s="7">
-        <f>P24/Z24</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE25" s="7" t="n">
+        <v>78.654322019064</v>
+      </c>
+      <c r="AF25" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:32">
       <c r="B26" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C26" s="2" t="n">
         <v>27436.34</v>
@@ -3294,20 +3252,18 @@
         <v>2032.32</v>
       </c>
       <c r="AD26" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE26" s="7">
-        <f>Q25/P25</f>
-        <v/>
-      </c>
-      <c r="AF26" s="7">
-        <f>P25/Z25</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE26" s="7" t="n">
+        <v>79.77238437825116</v>
+      </c>
+      <c r="AF26" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:32">
       <c r="B27" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C27" s="2" t="n">
         <v>6140.51</v>
@@ -3352,20 +3308,18 @@
         <v>454.85</v>
       </c>
       <c r="AD27" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE27" s="7">
-        <f>Q26/P26</f>
-        <v/>
-      </c>
-      <c r="AF27" s="7">
-        <f>P26/Z26</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE27" s="7" t="n">
+        <v>82.58966878325039</v>
+      </c>
+      <c r="AF27" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:32">
       <c r="B28" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C28" s="2" t="n">
         <v>7959.05</v>
@@ -3410,20 +3364,18 @@
         <v>589.5599999999999</v>
       </c>
       <c r="AD28" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE28" s="7">
-        <f>Q27/P27</f>
-        <v/>
-      </c>
-      <c r="AF28" s="7">
-        <f>P27/Z27</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE28" s="7" t="n">
+        <v>76.93010474893137</v>
+      </c>
+      <c r="AF28" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:32">
       <c r="B29" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C29" s="2" t="n">
         <v>35716.52</v>
@@ -3468,20 +3420,18 @@
         <v>2645.67</v>
       </c>
       <c r="AD29" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE29" s="7">
-        <f>Q28/P28</f>
-        <v/>
-      </c>
-      <c r="AF29" s="7">
-        <f>P28/Z28</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE29" s="7" t="n">
+        <v>77.04412573084802</v>
+      </c>
+      <c r="AF29" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:32">
       <c r="B30" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C30" s="2" t="n">
         <v>546218.72</v>
@@ -3529,20 +3479,18 @@
         <v>40460.65</v>
       </c>
       <c r="AD30" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE30" s="7">
-        <f>Q29/P29</f>
-        <v/>
-      </c>
-      <c r="AF30" s="7">
-        <f>P29/Z29</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE30" s="7" t="n">
+        <v>78.50008325876146</v>
+      </c>
+      <c r="AF30" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:32">
       <c r="B31" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C31" s="2" t="n">
         <v>16306.67</v>
@@ -3587,20 +3535,18 @@
         <v>1207.9</v>
       </c>
       <c r="AD31" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE31" s="7">
-        <f>Q30/P30</f>
-        <v/>
-      </c>
-      <c r="AF31" s="7">
-        <f>P30/Z30</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE31" s="7" t="n">
+        <v>77.11609924118521</v>
+      </c>
+      <c r="AF31" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:32">
       <c r="B32" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C32" s="2" t="n">
         <v>1682.46</v>
@@ -3645,20 +3591,18 @@
         <v>124.63</v>
       </c>
       <c r="AD32" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE32" s="7">
-        <f>Q31/P31</f>
-        <v/>
-      </c>
-      <c r="AF32" s="7">
-        <f>P31/Z31</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE32" s="7" t="n">
+        <v>81.37150466045273</v>
+      </c>
+      <c r="AF32" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:32">
       <c r="B33" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="C33" s="2" t="n">
         <v>28751.22</v>
@@ -3670,20 +3614,18 @@
         <v>2129.72</v>
       </c>
       <c r="AD33" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE33" s="7">
-        <f>Q32/P32</f>
-        <v/>
-      </c>
-      <c r="AF33" s="7">
-        <f>P32/Z32</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE33" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="AF33" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:32">
       <c r="B34" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C34" s="2" t="n">
         <v>26898.36</v>
@@ -3728,20 +3670,18 @@
         <v>1992.47</v>
       </c>
       <c r="AD34" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE34" s="7">
-        <f>Q33/P33</f>
-        <v/>
-      </c>
-      <c r="AF34" s="7">
-        <f>P33/Z33</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE34" s="7" t="n">
+        <v>76.39662710593886</v>
+      </c>
+      <c r="AF34" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:32">
       <c r="B35" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C35" s="2" t="n">
         <v>16298.61</v>
@@ -3786,20 +3726,18 @@
         <v>1207.3</v>
       </c>
       <c r="AD35" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE35" s="7">
-        <f>Q34/P34</f>
-        <v/>
-      </c>
-      <c r="AF35" s="7">
-        <f>P34/Z34</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE35" s="7" t="n">
+        <v>76.8125837825504</v>
+      </c>
+      <c r="AF35" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:32">
       <c r="B36" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C36" s="2" t="n">
         <v>119556.31</v>
@@ -3811,20 +3749,18 @@
         <v>8856.02</v>
       </c>
       <c r="AD36" t="s">
-        <v>106</v>
-      </c>
-      <c r="AE36" s="7">
-        <f>Q35/P35</f>
-        <v/>
-      </c>
-      <c r="AF36" s="7">
-        <f>P35/Z35</f>
-        <v/>
+        <v>107</v>
+      </c>
+      <c r="AE36" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="AF36" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:32">
       <c r="A37" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C37" s="2" t="n">
         <v>120.99</v>
@@ -3895,18 +3831,16 @@
       <c r="Z37" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="AE37" s="7">
-        <f>Q36/P36</f>
-        <v/>
-      </c>
-      <c r="AF37" s="7">
-        <f>P36/Z36</f>
-        <v/>
+      <c r="AE37" s="7" t="n">
+        <v>73.228285933897</v>
+      </c>
+      <c r="AF37" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="1:32">
       <c r="B38" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C38" s="2" t="n">
         <v>120.99</v>
@@ -3930,20 +3864,18 @@
         <v>8.960000000000001</v>
       </c>
       <c r="AD38" t="s">
-        <v>140</v>
-      </c>
-      <c r="AE38" s="7">
-        <f>Q37/P37</f>
-        <v/>
-      </c>
-      <c r="AF38" s="7">
-        <f>P37/Z37</f>
-        <v/>
+        <v>141</v>
+      </c>
+      <c r="AE38" s="7" t="n">
+        <v>73.228285933897</v>
+      </c>
+      <c r="AF38" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:32">
       <c r="A39" s="1" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C39" s="2" t="n">
         <v>1011.32</v>
@@ -4014,18 +3946,16 @@
       <c r="Z39" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="AE39" s="7">
-        <f>Q38/P38</f>
-        <v/>
-      </c>
-      <c r="AF39" s="7">
-        <f>P38/Z38</f>
-        <v/>
+      <c r="AE39" s="7" t="n">
+        <v>73.22691197691199</v>
+      </c>
+      <c r="AF39" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:32">
       <c r="B40" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C40" s="2" t="n">
         <v>1011.32</v>
@@ -4049,20 +3979,18 @@
         <v>74.91</v>
       </c>
       <c r="AD40" t="s">
-        <v>142</v>
-      </c>
-      <c r="AE40" s="7">
-        <f>Q39/P39</f>
-        <v/>
-      </c>
-      <c r="AF40" s="7">
-        <f>P39/Z39</f>
-        <v/>
+        <v>143</v>
+      </c>
+      <c r="AE40" s="7" t="n">
+        <v>73.22691197691199</v>
+      </c>
+      <c r="AF40" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:32">
       <c r="A41" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C41" s="2" t="n">
         <v>693.46</v>
@@ -4133,18 +4061,16 @@
       <c r="Z41" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="AE41" s="7">
-        <f>Q40/P40</f>
-        <v/>
-      </c>
-      <c r="AF41" s="7">
-        <f>P40/Z40</f>
-        <v/>
+      <c r="AE41" s="7" t="n">
+        <v>73.22745901639344</v>
+      </c>
+      <c r="AF41" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:32">
       <c r="B42" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C42" s="2" t="n">
         <v>693.46</v>
@@ -4168,20 +4094,18 @@
         <v>51.37</v>
       </c>
       <c r="AD42" t="s">
-        <v>144</v>
-      </c>
-      <c r="AE42" s="7">
-        <f>Q41/P41</f>
-        <v/>
-      </c>
-      <c r="AF42" s="7">
-        <f>P41/Z41</f>
-        <v/>
+        <v>145</v>
+      </c>
+      <c r="AE42" s="7" t="n">
+        <v>73.22745901639344</v>
+      </c>
+      <c r="AF42" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:32">
       <c r="A43" s="1" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C43" s="2" t="n">
         <v>-35678.73</v>
@@ -4252,18 +4176,16 @@
       <c r="Z43" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="AE43" s="7">
-        <f>Q42/P42</f>
-        <v/>
-      </c>
-      <c r="AF43" s="7">
-        <f>P42/Z42</f>
-        <v/>
+      <c r="AE43" s="7" t="n">
+        <v>73.22718423043165</v>
+      </c>
+      <c r="AF43" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="44" spans="1:32">
       <c r="B44" s="1" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C44" s="2" t="n">
         <v>-35678.73</v>
@@ -4287,20 +4209,18 @@
         <v>-2642.87</v>
       </c>
       <c r="AD44" t="s">
-        <v>146</v>
-      </c>
-      <c r="AE44" s="7">
-        <f>Q43/P43</f>
-        <v/>
-      </c>
-      <c r="AF44" s="7">
-        <f>P43/Z43</f>
-        <v/>
+        <v>147</v>
+      </c>
+      <c r="AE44" s="7" t="n">
+        <v>73.22718423043165</v>
+      </c>
+      <c r="AF44" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:32">
       <c r="A45" s="1" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C45" s="2" t="n">
         <v>135355.04</v>
@@ -4371,18 +4291,16 @@
       <c r="Z45" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="AE45" s="7">
-        <f>Q44/P44</f>
-        <v/>
-      </c>
-      <c r="AF45" s="7">
-        <f>P44/Z44</f>
-        <v/>
+      <c r="AE45" s="7" t="n">
+        <v>73.22718895266335</v>
+      </c>
+      <c r="AF45" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:32">
       <c r="B46" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C46" s="2" t="n">
         <v>42725.71</v>
@@ -4406,20 +4324,18 @@
         <v>3164.87</v>
       </c>
       <c r="AD46" t="s">
-        <v>148</v>
-      </c>
-      <c r="AE46" s="7">
-        <f>Q45/P45</f>
-        <v/>
-      </c>
-      <c r="AF46" s="7">
-        <f>P45/Z45</f>
-        <v/>
+        <v>149</v>
+      </c>
+      <c r="AE46" s="7" t="n">
+        <v>73.22718665264874</v>
+      </c>
+      <c r="AF46" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:32">
       <c r="B47" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C47" s="2" t="n">
         <v>92629.33</v>
@@ -4443,20 +4359,18 @@
         <v>6861.43</v>
       </c>
       <c r="AD47" t="s">
-        <v>148</v>
-      </c>
-      <c r="AE47" s="7">
-        <f>Q46/P46</f>
-        <v/>
-      </c>
-      <c r="AF47" s="7">
-        <f>P46/Z46</f>
-        <v/>
+        <v>149</v>
+      </c>
+      <c r="AE47" s="7" t="n">
+        <v>73.22719000369561</v>
+      </c>
+      <c r="AF47" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:32">
       <c r="A48" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C48" s="2" t="n">
         <v>-50548.75</v>
@@ -4527,18 +4441,16 @@
       <c r="Z48" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="AE48" s="7">
-        <f>Q47/P47</f>
-        <v/>
-      </c>
-      <c r="AF48" s="7">
-        <f>P47/Z47</f>
-        <v/>
+      <c r="AE48" s="7" t="n">
+        <v>73.2271939262106</v>
+      </c>
+      <c r="AF48" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:32">
       <c r="B49" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C49" s="2" t="n">
         <v>-50548.75</v>
@@ -4562,20 +4474,18 @@
         <v>-3744.35</v>
       </c>
       <c r="AD49" t="s">
-        <v>150</v>
-      </c>
-      <c r="AE49" s="7">
-        <f>Q48/P48</f>
-        <v/>
-      </c>
-      <c r="AF49" s="7">
-        <f>P48/Z48</f>
-        <v/>
+        <v>151</v>
+      </c>
+      <c r="AE49" s="7" t="n">
+        <v>73.2271939262106</v>
+      </c>
+      <c r="AF49" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:32">
       <c r="B50" s="1" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C50" s="2" t="n">
         <v>6317922.71</v>
@@ -4625,13 +4535,11 @@
       <c r="W50" s="4" t="n">
         <v>467994.2</v>
       </c>
-      <c r="AE50" s="7">
-        <f>Q49/P49</f>
-        <v/>
-      </c>
-      <c r="AF50" s="7">
-        <f>P49/Z49</f>
-        <v/>
+      <c r="AE50" s="7" t="n">
+        <v>78.64099765663585</v>
+      </c>
+      <c r="AF50" s="7" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -4643,4 +4551,22 @@
   <pageMargins bottom="1.9" footer="0.5" header="0.5" left="1.8" right="1.8" top="1.9"/>
   <pageSetup fitToHeight="0" fitToWidth="0" horizontalDpi="0" orientation="portrait" paperSize="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:S43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.75"/>
+  <sheetData/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>